<commit_message>
20210719 Add kubernates document
</commit_message>
<xml_diff>
--- a/Docker.xlsx
+++ b/Docker.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\資料\勉強\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\jeus-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6000" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="install" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,8 @@
     <sheet name="cgroup error" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
     <sheet name="port forward" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
-    <sheet name="volume設定" sheetId="7" r:id="rId8"/>
-    <sheet name="payara-oracle連結" sheetId="8" r:id="rId9"/>
+    <sheet name="volume設定" sheetId="7" r:id="rId7"/>
+    <sheet name="payara-oracle連結" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -5199,7 +5198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E292"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
@@ -5297,7 +5296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -5440,7 +5439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B33:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
@@ -5501,24 +5500,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M42" sqref="M40:M42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B125"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W126" sqref="W126"/>
     </sheetView>
   </sheetViews>
@@ -5567,11 +5551,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S88"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W71" sqref="W71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added action for when Veigrant times out.
</commit_message>
<xml_diff>
--- a/Docker.xlsx
+++ b/Docker.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="install" sheetId="1" r:id="rId1"/>
     <sheet name="commands" sheetId="9" r:id="rId2"/>
     <sheet name="Docker-DeskTop" sheetId="6" r:id="rId3"/>
     <sheet name="host-only error" sheetId="2" r:id="rId4"/>
-    <sheet name="cgroup error" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
-    <sheet name="port forward" sheetId="4" r:id="rId7"/>
-    <sheet name="volume設定" sheetId="7" r:id="rId8"/>
-    <sheet name="payara-oracle連結" sheetId="8" r:id="rId9"/>
+    <sheet name="Waiting no response" sheetId="10" r:id="rId5"/>
+    <sheet name="cgroup error" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
+    <sheet name="port forward" sheetId="4" r:id="rId8"/>
+    <sheet name="volume設定" sheetId="7" r:id="rId9"/>
+    <sheet name="payara-oracle連結" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="175">
   <si>
     <t>https://docs.docker.com/toolbox/toolbox_install_windows/</t>
   </si>
@@ -1432,12 +1434,12 @@
   <si>
     <t>-&gt; nginx イメージ一律削除</t>
     <rPh sb="14" eb="16">
-      <t>イチリツ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>サクジョ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
+      <t>イチリツサクジョ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>(default) Waiting for an IP...</t>
   </si>
 </sst>
 </file>
@@ -1609,10 +1611,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3208,6 +3210,49 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>65219</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1005840"/>
+          <a:ext cx="11647619" cy="6085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3283,7 +3328,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3326,7 +3371,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3795,7 +3840,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5730,7 +5775,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -6317,11 +6362,184 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:S88"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W71" sqref="W71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S84" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S85" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S86" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S87" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:AY127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
@@ -6432,254 +6650,254 @@
       </c>
     </row>
     <row r="27" spans="5:51" x14ac:dyDescent="0.2">
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11" t="s">
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11" t="s">
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AM27" s="11"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="11"/>
-      <c r="AQ27" s="11"/>
-      <c r="AR27" s="11"/>
-      <c r="AS27" s="11"/>
-      <c r="AT27" s="11"/>
-      <c r="AU27" s="11"/>
-      <c r="AV27" s="11"/>
-      <c r="AW27" s="11"/>
-      <c r="AX27" s="11"/>
-      <c r="AY27" s="11"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="12"/>
+      <c r="AJ27" s="12"/>
+      <c r="AK27" s="12"/>
+      <c r="AL27" s="12"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="12"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="12"/>
+      <c r="AS27" s="12"/>
+      <c r="AT27" s="12"/>
+      <c r="AU27" s="12"/>
+      <c r="AV27" s="12"/>
+      <c r="AW27" s="12"/>
+      <c r="AX27" s="12"/>
+      <c r="AY27" s="12"/>
     </row>
     <row r="28" spans="5:51" x14ac:dyDescent="0.2">
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12" t="s">
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="12"/>
-      <c r="AC28" s="12"/>
-      <c r="AD28" s="12"/>
-      <c r="AE28" s="12" t="s">
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AF28" s="12"/>
-      <c r="AG28" s="12"/>
-      <c r="AH28" s="12"/>
-      <c r="AI28" s="12"/>
-      <c r="AJ28" s="12"/>
-      <c r="AK28" s="12"/>
-      <c r="AL28" s="12"/>
-      <c r="AM28" s="12"/>
-      <c r="AN28" s="12"/>
-      <c r="AO28" s="12"/>
-      <c r="AP28" s="12"/>
-      <c r="AQ28" s="12"/>
-      <c r="AR28" s="12"/>
-      <c r="AS28" s="12"/>
-      <c r="AT28" s="12"/>
-      <c r="AU28" s="12"/>
-      <c r="AV28" s="12"/>
-      <c r="AW28" s="12"/>
-      <c r="AX28" s="12"/>
-      <c r="AY28" s="12"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
+      <c r="AM28" s="11"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="11"/>
+      <c r="AQ28" s="11"/>
+      <c r="AR28" s="11"/>
+      <c r="AS28" s="11"/>
+      <c r="AT28" s="11"/>
+      <c r="AU28" s="11"/>
+      <c r="AV28" s="11"/>
+      <c r="AW28" s="11"/>
+      <c r="AX28" s="11"/>
+      <c r="AY28" s="11"/>
     </row>
     <row r="29" spans="5:51" x14ac:dyDescent="0.2">
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12" t="s">
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="12"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12" t="s">
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
-      <c r="AH29" s="12"/>
-      <c r="AI29" s="12"/>
-      <c r="AJ29" s="12"/>
-      <c r="AK29" s="12"/>
-      <c r="AL29" s="12"/>
-      <c r="AM29" s="12"/>
-      <c r="AN29" s="12"/>
-      <c r="AO29" s="12"/>
-      <c r="AP29" s="12"/>
-      <c r="AQ29" s="12"/>
-      <c r="AR29" s="12"/>
-      <c r="AS29" s="12"/>
-      <c r="AT29" s="12"/>
-      <c r="AU29" s="12"/>
-      <c r="AV29" s="12"/>
-      <c r="AW29" s="12"/>
-      <c r="AX29" s="12"/>
-      <c r="AY29" s="12"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+      <c r="AH29" s="11"/>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="11"/>
+      <c r="AM29" s="11"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="11"/>
+      <c r="AP29" s="11"/>
+      <c r="AQ29" s="11"/>
+      <c r="AR29" s="11"/>
+      <c r="AS29" s="11"/>
+      <c r="AT29" s="11"/>
+      <c r="AU29" s="11"/>
+      <c r="AV29" s="11"/>
+      <c r="AW29" s="11"/>
+      <c r="AX29" s="11"/>
+      <c r="AY29" s="11"/>
     </row>
     <row r="30" spans="5:51" x14ac:dyDescent="0.2">
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12" t="s">
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
-      <c r="U30" s="12"/>
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="12"/>
-      <c r="Y30" s="12"/>
-      <c r="Z30" s="12"/>
-      <c r="AA30" s="12"/>
-      <c r="AB30" s="12"/>
-      <c r="AC30" s="12"/>
-      <c r="AD30" s="12"/>
-      <c r="AE30" s="12" t="s">
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AF30" s="12"/>
-      <c r="AG30" s="12"/>
-      <c r="AH30" s="12"/>
-      <c r="AI30" s="12"/>
-      <c r="AJ30" s="12"/>
-      <c r="AK30" s="12"/>
-      <c r="AL30" s="12"/>
-      <c r="AM30" s="12"/>
-      <c r="AN30" s="12"/>
-      <c r="AO30" s="12"/>
-      <c r="AP30" s="12"/>
-      <c r="AQ30" s="12"/>
-      <c r="AR30" s="12"/>
-      <c r="AS30" s="12"/>
-      <c r="AT30" s="12"/>
-      <c r="AU30" s="12"/>
-      <c r="AV30" s="12"/>
-      <c r="AW30" s="12"/>
-      <c r="AX30" s="12"/>
-      <c r="AY30" s="12"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="11"/>
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="11"/>
+      <c r="AM30" s="11"/>
+      <c r="AN30" s="11"/>
+      <c r="AO30" s="11"/>
+      <c r="AP30" s="11"/>
+      <c r="AQ30" s="11"/>
+      <c r="AR30" s="11"/>
+      <c r="AS30" s="11"/>
+      <c r="AT30" s="11"/>
+      <c r="AU30" s="11"/>
+      <c r="AV30" s="11"/>
+      <c r="AW30" s="11"/>
+      <c r="AX30" s="11"/>
+      <c r="AY30" s="11"/>
     </row>
     <row r="31" spans="5:51" x14ac:dyDescent="0.2">
-      <c r="J31" s="12" t="s">
+      <c r="J31" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12" t="s">
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
-      <c r="U31" s="12"/>
-      <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="12"/>
-      <c r="Y31" s="12"/>
-      <c r="Z31" s="12"/>
-      <c r="AA31" s="12"/>
-      <c r="AB31" s="12"/>
-      <c r="AC31" s="12"/>
-      <c r="AD31" s="12"/>
-      <c r="AE31" s="12" t="s">
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
-      <c r="AH31" s="12"/>
-      <c r="AI31" s="12"/>
-      <c r="AJ31" s="12"/>
-      <c r="AK31" s="12"/>
-      <c r="AL31" s="12"/>
-      <c r="AM31" s="12"/>
-      <c r="AN31" s="12"/>
-      <c r="AO31" s="12"/>
-      <c r="AP31" s="12"/>
-      <c r="AQ31" s="12"/>
-      <c r="AR31" s="12"/>
-      <c r="AS31" s="12"/>
-      <c r="AT31" s="12"/>
-      <c r="AU31" s="12"/>
-      <c r="AV31" s="12"/>
-      <c r="AW31" s="12"/>
-      <c r="AX31" s="12"/>
-      <c r="AY31" s="12"/>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="11"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="11"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="11"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="11"/>
+      <c r="AR31" s="11"/>
+      <c r="AS31" s="11"/>
+      <c r="AT31" s="11"/>
+      <c r="AU31" s="11"/>
+      <c r="AV31" s="11"/>
+      <c r="AW31" s="11"/>
+      <c r="AX31" s="11"/>
+      <c r="AY31" s="11"/>
     </row>
     <row r="32" spans="5:51" x14ac:dyDescent="0.2">
       <c r="J32" s="10"/>
@@ -7306,6 +7524,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J27:Q27"/>
+    <mergeCell ref="R27:AD27"/>
+    <mergeCell ref="AE27:AY27"/>
+    <mergeCell ref="J28:Q28"/>
+    <mergeCell ref="R28:AD28"/>
+    <mergeCell ref="AE28:AY28"/>
     <mergeCell ref="J31:Q31"/>
     <mergeCell ref="R31:AD31"/>
     <mergeCell ref="AE31:AY31"/>
@@ -7315,12 +7539,6 @@
     <mergeCell ref="J30:Q30"/>
     <mergeCell ref="R30:AD30"/>
     <mergeCell ref="AE30:AY30"/>
-    <mergeCell ref="J27:Q27"/>
-    <mergeCell ref="R27:AD27"/>
-    <mergeCell ref="AE27:AY27"/>
-    <mergeCell ref="J28:Q28"/>
-    <mergeCell ref="R28:AD28"/>
-    <mergeCell ref="AE28:AY28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7484,6 +7702,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7498,7 +7753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B33:B38"/>
   <sheetViews>
@@ -7545,7 +7800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7561,7 +7816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B125"/>
   <sheetViews>
@@ -7612,177 +7867,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S88"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W71" sqref="W71"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="84" spans="19:19" x14ac:dyDescent="0.2">
-      <c r="S84" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="19:19" x14ac:dyDescent="0.2">
-      <c r="S85" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="86" spans="19:19" x14ac:dyDescent="0.2">
-      <c r="S86" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="87" spans="19:19" x14ac:dyDescent="0.2">
-      <c r="S87" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="88" spans="19:19" x14ac:dyDescent="0.2">
-      <c r="S88" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>